<commit_message>
Added www interface and cleaning up api
</commit_message>
<xml_diff>
--- a/Documentation/Database design.xlsx
+++ b/Documentation/Database design.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frode/git/BluePrism-Hugin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frode/git/BluePrism-Hugin/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F995EFF-B8E7-BA41-AED0-B0DB76698D0F}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE0A7B4-45C9-9E45-AEE0-97998104643A}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20900" yWindow="7640" windowWidth="18720" windowHeight="12220" xr2:uid="{368F9A67-AE22-4ECC-A85F-2330F35214E9}"/>
+    <workbookView xWindow="3340" yWindow="2620" windowWidth="18720" windowHeight="12220" xr2:uid="{368F9A67-AE22-4ECC-A85F-2330F35214E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="74">
   <si>
     <t>ProcessTable</t>
   </si>
@@ -245,13 +245,16 @@
   </si>
   <si>
     <t>Hypercare</t>
+  </si>
+  <si>
+    <t>REST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +285,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -389,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -405,6 +416,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9237427-E118-46BA-A5B1-344C350CCA7D}">
-  <dimension ref="B1:N23"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1008,7 +1020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
@@ -1016,7 +1028,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>4</v>
       </c>
@@ -1030,7 +1042,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
         <v>16</v>
@@ -1042,7 +1054,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
         <v>4</v>
       </c>
@@ -1056,7 +1068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
         <v>28</v>
@@ -1068,7 +1080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
         <v>26</v>
@@ -1080,7 +1092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" s="7"/>
       <c r="C23" s="8" t="s">
         <v>41</v>
@@ -1090,6 +1102,26 @@
       </c>
       <c r="E23" s="8" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>